<commit_message>
waiting to add file path, client email
</commit_message>
<xml_diff>
--- a/invoices.xlsx
+++ b/invoices.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,29 +471,65 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2023-11-23</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2023-11-30</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>40.25</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G2" t="n">
+        <v>42.3</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Unpaid</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>John Smith</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>us-001</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2019-02-11</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2019-11-02</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>2019-02-26</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="E3" t="n">
         <v>145</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F3" t="n">
         <v>9.06</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G3" t="n">
         <v>154.06</v>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Unpaid</t>
         </is>

</xml_diff>